<commit_message>
SEC and function updates
</commit_message>
<xml_diff>
--- a/notes/schools.xlsx
+++ b/notes/schools.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="140">
   <si>
     <t>school</t>
   </si>
@@ -318,6 +318,135 @@
   </si>
   <si>
     <t xml:space="preserve">http://www.hokiesports.com/football/players/ </t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>LSU</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Ole Miss</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M</t>
+  </si>
+  <si>
+    <t>Vanderbilt</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>alabama.py</t>
+  </si>
+  <si>
+    <t>arkansas.py</t>
+  </si>
+  <si>
+    <t>auburn.py</t>
+  </si>
+  <si>
+    <t>florida.py</t>
+  </si>
+  <si>
+    <t>georgia.py</t>
+  </si>
+  <si>
+    <t>kentucky.py</t>
+  </si>
+  <si>
+    <t>lsu.py</t>
+  </si>
+  <si>
+    <t>missouri.py</t>
+  </si>
+  <si>
+    <t>tennessee.py</t>
+  </si>
+  <si>
+    <t>vanderbilt.py</t>
+  </si>
+  <si>
+    <t>miss_state.py</t>
+  </si>
+  <si>
+    <t>Miss. State</t>
+  </si>
+  <si>
+    <t>ole_miss.py</t>
+  </si>
+  <si>
+    <t>south_carolina.py</t>
+  </si>
+  <si>
+    <t>texas_am.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.rolltide.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.arkansasrazorbacks.com/sport/m-footbl/roster/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.auburntigers.com/sports/m-footbl/mtt/aub-m-footbl-mtt.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://floridagators.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://georgiadogs.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ukathletics.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.lsusports.net/SportSelect.dbml?DB_OEM_ID=5200&amp;SPID=2164&amp;SPSID=27812 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hailstate.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mutigers.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.olemisssports.com/sports/m-footbl/mtt/ole-m-footbl-mtt.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.gamecocksonline.com/sports/m-footbl/mtt/scar-m-footbl-mtt.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://utsports.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://12thman.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t>http://www.vucommodores.com/sports/m-footbl/mtt/vand-m-footbl-mtt.html</t>
   </si>
 </sst>
 </file>
@@ -648,12 +777,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,6 +1572,370 @@
       </c>
       <c r="H30" s="2" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>43207</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>43207</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>43207</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>43207</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>43207</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>43208</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>43206</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>43208</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1476,6 +1969,20 @@
     <hyperlink ref="H28" r:id="rId27"/>
     <hyperlink ref="H30" r:id="rId28"/>
     <hyperlink ref="H29" r:id="rId29"/>
+    <hyperlink ref="H31" r:id="rId30"/>
+    <hyperlink ref="H32" r:id="rId31"/>
+    <hyperlink ref="H33" r:id="rId32"/>
+    <hyperlink ref="H34" r:id="rId33"/>
+    <hyperlink ref="H35" r:id="rId34"/>
+    <hyperlink ref="H36" r:id="rId35"/>
+    <hyperlink ref="H37" r:id="rId36"/>
+    <hyperlink ref="H38" r:id="rId37"/>
+    <hyperlink ref="H39" r:id="rId38"/>
+    <hyperlink ref="H40" r:id="rId39"/>
+    <hyperlink ref="H41" r:id="rId40"/>
+    <hyperlink ref="H42" r:id="rId41"/>
+    <hyperlink ref="H43" r:id="rId42"/>
+    <hyperlink ref="H44" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Big 12 and updates
</commit_message>
<xml_diff>
--- a/notes/schools.xlsx
+++ b/notes/schools.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="171">
   <si>
     <t>school</t>
   </si>
@@ -447,6 +447,99 @@
   </si>
   <si>
     <t>http://www.vucommodores.com/sports/m-footbl/mtt/vand-m-footbl-mtt.html</t>
+  </si>
+  <si>
+    <t>Baylor</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kansas State</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oklahoma State</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Big 12</t>
+  </si>
+  <si>
+    <t>baylor.py</t>
+  </si>
+  <si>
+    <t>iowa state.py</t>
+  </si>
+  <si>
+    <t>kansas.py</t>
+  </si>
+  <si>
+    <t>oklahoma.py</t>
+  </si>
+  <si>
+    <t>tcu.py</t>
+  </si>
+  <si>
+    <t>texas.py</t>
+  </si>
+  <si>
+    <t>kansas_state.py</t>
+  </si>
+  <si>
+    <t>oklahoma_state.py</t>
+  </si>
+  <si>
+    <t>texas_tech.py</t>
+  </si>
+  <si>
+    <t>west_virginia.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.baylorbears.com/sports/m-footbl/mtt/bay-m-footbl-mtt.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cyclones.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kuathletics.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.kstatesports.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.soonersports.com/SportSelect.dbml?DB_OEM_ID=31000&amp;SPID=127245&amp;SPSID=750326 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://okstate.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.gofrogs.com/sports/m-footbl/mtt/tcu-m-footbl-mtt.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://texassports.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://texastech.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://wvusports.com/roster.aspx?path=football </t>
   </si>
 </sst>
 </file>
@@ -777,12 +870,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1936,6 +2029,266 @@
       </c>
       <c r="H44" s="2" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>154</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>43211</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>43212</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>43212</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>43212</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1983,6 +2336,16 @@
     <hyperlink ref="H42" r:id="rId41"/>
     <hyperlink ref="H43" r:id="rId42"/>
     <hyperlink ref="H44" r:id="rId43"/>
+    <hyperlink ref="H45" r:id="rId44"/>
+    <hyperlink ref="H46" r:id="rId45"/>
+    <hyperlink ref="H47" r:id="rId46"/>
+    <hyperlink ref="H48" r:id="rId47"/>
+    <hyperlink ref="H49" r:id="rId48"/>
+    <hyperlink ref="H50" r:id="rId49"/>
+    <hyperlink ref="H51" r:id="rId50"/>
+    <hyperlink ref="H52" r:id="rId51"/>
+    <hyperlink ref="H53" r:id="rId52"/>
+    <hyperlink ref="H54" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pac-12 and new ul template
</commit_message>
<xml_diff>
--- a/notes/schools.xlsx
+++ b/notes/schools.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="208">
   <si>
     <t>school</t>
   </si>
@@ -540,6 +540,117 @@
   </si>
   <si>
     <t xml:space="preserve">https://wvusports.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arizona State</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Oregon State</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Washington State</t>
+  </si>
+  <si>
+    <t>Pac-12</t>
+  </si>
+  <si>
+    <t>arizona.py</t>
+  </si>
+  <si>
+    <t>cal.py</t>
+  </si>
+  <si>
+    <t>colorado.py</t>
+  </si>
+  <si>
+    <t>oregon.py</t>
+  </si>
+  <si>
+    <t>stanford.py</t>
+  </si>
+  <si>
+    <t>ucla.py</t>
+  </si>
+  <si>
+    <t>usc.py</t>
+  </si>
+  <si>
+    <t>utah.py</t>
+  </si>
+  <si>
+    <t>washington.py</t>
+  </si>
+  <si>
+    <t>arizona_state.py</t>
+  </si>
+  <si>
+    <t>oregon_state.py</t>
+  </si>
+  <si>
+    <t>washington_state.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://arizonawildcats.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://thesundevils.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://calbears.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cubuffs.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://goducks.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://osubeavers.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gostanford.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://uclabruins.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://usctrojans.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://utahutes.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gohuskies.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://wsucougars.com/roster.aspx?path=football </t>
   </si>
 </sst>
 </file>
@@ -870,19 +981,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="99.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2289,6 +2400,318 @@
       </c>
       <c r="H54" s="2" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>43215</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" t="s">
+        <v>193</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>43215</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3">
+        <v>43231</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
+        <v>43231</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" t="s">
+        <v>183</v>
+      </c>
+      <c r="C62" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" t="s">
+        <v>183</v>
+      </c>
+      <c r="C64" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>182</v>
+      </c>
+      <c r="B66" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>43232</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2346,6 +2769,18 @@
     <hyperlink ref="H52" r:id="rId51"/>
     <hyperlink ref="H53" r:id="rId52"/>
     <hyperlink ref="H54" r:id="rId53"/>
+    <hyperlink ref="H55" r:id="rId54"/>
+    <hyperlink ref="H56" r:id="rId55"/>
+    <hyperlink ref="H57" r:id="rId56"/>
+    <hyperlink ref="H58" r:id="rId57"/>
+    <hyperlink ref="H59" r:id="rId58"/>
+    <hyperlink ref="H60" r:id="rId59"/>
+    <hyperlink ref="H61" r:id="rId60"/>
+    <hyperlink ref="H62" r:id="rId61"/>
+    <hyperlink ref="H63" r:id="rId62"/>
+    <hyperlink ref="H64" r:id="rId63"/>
+    <hyperlink ref="H65" r:id="rId64"/>
+    <hyperlink ref="H66" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaning functions and final rosters
</commit_message>
<xml_diff>
--- a/notes/schools.xlsx
+++ b/notes/schools.xlsx
@@ -485,9 +485,6 @@
     <t>baylor.py</t>
   </si>
   <si>
-    <t>iowa state.py</t>
-  </si>
-  <si>
     <t>kansas.py</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://wsucougars.com/roster.aspx?path=football </t>
+  </si>
+  <si>
+    <t>iowa_state.py</t>
   </si>
 </sst>
 </file>
@@ -984,9 +984,9 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>43204</v>
+        <v>43233</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>85</v>
@@ -2165,7 +2165,7 @@
         <v>43211</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2176,7 +2176,7 @@
         <v>150</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>43232</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2202,7 +2202,7 @@
         <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2217,7 +2217,7 @@
         <v>43232</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2228,7 +2228,7 @@
         <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2243,7 +2243,7 @@
         <v>43232</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2254,7 +2254,7 @@
         <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2269,7 +2269,7 @@
         <v>43211</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -2280,7 +2280,7 @@
         <v>150</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2295,7 +2295,7 @@
         <v>43211</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -2306,7 +2306,7 @@
         <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2321,7 +2321,7 @@
         <v>43211</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -2332,7 +2332,7 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2344,10 +2344,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="3">
-        <v>43232</v>
+        <v>43233</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -2358,7 +2358,7 @@
         <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2373,7 +2373,7 @@
         <v>43232</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -2384,7 +2384,7 @@
         <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2399,19 +2399,19 @@
         <v>43232</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" t="s">
         <v>183</v>
       </c>
-      <c r="C55" t="s">
-        <v>184</v>
-      </c>
       <c r="D55">
         <v>0</v>
       </c>
@@ -2425,18 +2425,18 @@
         <v>43232</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2451,18 +2451,18 @@
         <v>43232</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2477,18 +2477,18 @@
         <v>43231</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2503,18 +2503,18 @@
         <v>43231</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2529,18 +2529,18 @@
         <v>43232</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2555,18 +2555,18 @@
         <v>43232</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2581,18 +2581,18 @@
         <v>43232</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2607,18 +2607,18 @@
         <v>43232</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2633,18 +2633,18 @@
         <v>43232</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2659,18 +2659,18 @@
         <v>43232</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C65" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2685,18 +2685,18 @@
         <v>43232</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" t="s">
         <v>182</v>
       </c>
-      <c r="B66" t="s">
-        <v>183</v>
-      </c>
       <c r="C66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2711,7 +2711,7 @@
         <v>43232</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add high schools and scrape methods
</commit_message>
<xml_diff>
--- a/notes/schools.xlsx
+++ b/notes/schools.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$66</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -317,9 +317,6 @@
     <t xml:space="preserve">http://www.wakeforestsports.com/sports/m-footbl/mtt/wake-m-footbl-mtt.html </t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.hokiesports.com/football/players/ </t>
-  </si>
-  <si>
     <t>Alabama</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t>iowa_state.py</t>
+  </si>
+  <si>
+    <t>https://hokiesports.com/roster.aspx?path=football</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>39</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>40</v>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="3">
-        <v>43200</v>
+        <v>43280</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>41</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>43</v>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>42</v>
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>44</v>
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>43200</v>
+        <v>43280</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>45</v>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>46</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>47</v>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>48</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>10</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>49</v>
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>43200</v>
+        <v>43277</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>50</v>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>82</v>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>43204</v>
+        <v>43280</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>83</v>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>43204</v>
+        <v>43280</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>84</v>
@@ -1486,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>43204</v>
+        <v>43277</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>87</v>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <v>43204</v>
+        <v>43277</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>86</v>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <v>43233</v>
+        <v>43277</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>85</v>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>88</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="3">
-        <v>43204</v>
+        <v>43277</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>89</v>
@@ -1616,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>90</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="3">
-        <v>43205</v>
+        <v>43277</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>91</v>
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>92</v>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>93</v>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="3">
-        <v>43205</v>
+        <v>43277</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>94</v>
@@ -1746,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="3">
-        <v>43205</v>
+        <v>43277</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>95</v>
@@ -1780,14 +1780,14 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
         <v>110</v>
       </c>
-      <c r="C31" t="s">
-        <v>111</v>
-      </c>
       <c r="D31">
         <v>0</v>
       </c>
@@ -1798,21 +1798,21 @@
         <v>0</v>
       </c>
       <c r="G31" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1824,21 +1824,21 @@
         <v>0</v>
       </c>
       <c r="G32" s="3">
-        <v>43207</v>
+        <v>43277</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1850,47 +1850,47 @@
         <v>0</v>
       </c>
       <c r="G33" s="3">
-        <v>43207</v>
+        <v>43277</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34" s="3">
-        <v>43207</v>
+        <v>43277</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1902,21 +1902,21 @@
         <v>0</v>
       </c>
       <c r="G35" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1928,21 +1928,21 @@
         <v>0</v>
       </c>
       <c r="G36" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1954,21 +1954,21 @@
         <v>1</v>
       </c>
       <c r="G37" s="3">
-        <v>43207</v>
+        <v>43280</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1980,21 +1980,21 @@
         <v>0</v>
       </c>
       <c r="G38" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2006,21 +2006,21 @@
         <v>0</v>
       </c>
       <c r="G39" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2032,21 +2032,21 @@
         <v>0</v>
       </c>
       <c r="G40" s="3">
-        <v>43207</v>
+        <v>43277</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2058,21 +2058,21 @@
         <v>0</v>
       </c>
       <c r="G41" s="3">
-        <v>43208</v>
+        <v>43277</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2084,21 +2084,21 @@
         <v>0</v>
       </c>
       <c r="G42" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2110,21 +2110,21 @@
         <v>0</v>
       </c>
       <c r="G43" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
         <v>109</v>
       </c>
-      <c r="B44" t="s">
-        <v>110</v>
-      </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2136,22 +2136,22 @@
         <v>0</v>
       </c>
       <c r="G44" s="3">
-        <v>43208</v>
+        <v>43277</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" t="s">
         <v>150</v>
       </c>
-      <c r="C45" t="s">
-        <v>151</v>
-      </c>
       <c r="D45">
         <v>1</v>
       </c>
@@ -2162,21 +2162,21 @@
         <v>0</v>
       </c>
       <c r="G45" s="3">
-        <v>43211</v>
+        <v>43277</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2188,21 +2188,21 @@
         <v>0</v>
       </c>
       <c r="G46" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2214,21 +2214,21 @@
         <v>0</v>
       </c>
       <c r="G47" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2240,21 +2240,21 @@
         <v>0</v>
       </c>
       <c r="G48" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2266,21 +2266,21 @@
         <v>1</v>
       </c>
       <c r="G49" s="3">
-        <v>43211</v>
+        <v>43280</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2292,21 +2292,21 @@
         <v>0</v>
       </c>
       <c r="G50" s="3">
-        <v>43211</v>
+        <v>43277</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2318,21 +2318,21 @@
         <v>0</v>
       </c>
       <c r="G51" s="3">
-        <v>43211</v>
+        <v>43277</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2344,21 +2344,21 @@
         <v>0</v>
       </c>
       <c r="G52" s="3">
-        <v>43233</v>
+        <v>43277</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2370,21 +2370,21 @@
         <v>0</v>
       </c>
       <c r="G53" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" t="s">
         <v>149</v>
       </c>
-      <c r="B54" t="s">
-        <v>150</v>
-      </c>
       <c r="C54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2396,22 +2396,22 @@
         <v>0</v>
       </c>
       <c r="G54" s="3">
-        <v>43232</v>
+        <v>43277</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" t="s">
         <v>182</v>
       </c>
-      <c r="C55" t="s">
-        <v>183</v>
-      </c>
       <c r="D55">
         <v>0</v>
       </c>
@@ -2422,21 +2422,21 @@
         <v>0</v>
       </c>
       <c r="G55" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2448,21 +2448,21 @@
         <v>0</v>
       </c>
       <c r="G56" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2474,21 +2474,21 @@
         <v>0</v>
       </c>
       <c r="G57" s="3">
-        <v>43231</v>
+        <v>43280</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2500,21 +2500,21 @@
         <v>0</v>
       </c>
       <c r="G58" s="3">
-        <v>43231</v>
+        <v>43280</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2526,21 +2526,21 @@
         <v>0</v>
       </c>
       <c r="G59" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2552,21 +2552,21 @@
         <v>0</v>
       </c>
       <c r="G60" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2578,21 +2578,21 @@
         <v>0</v>
       </c>
       <c r="G61" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B62" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2604,21 +2604,21 @@
         <v>0</v>
       </c>
       <c r="G62" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2630,21 +2630,21 @@
         <v>0</v>
       </c>
       <c r="G63" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2656,21 +2656,21 @@
         <v>0</v>
       </c>
       <c r="G64" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2682,21 +2682,21 @@
         <v>0</v>
       </c>
       <c r="G65" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" t="s">
         <v>181</v>
       </c>
-      <c r="B66" t="s">
-        <v>182</v>
-      </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2708,10 +2708,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="3">
-        <v>43232</v>
+        <v>43280</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2744,43 +2744,43 @@
     <hyperlink ref="H27" r:id="rId26"/>
     <hyperlink ref="H28" r:id="rId27"/>
     <hyperlink ref="H30" r:id="rId28"/>
-    <hyperlink ref="H29" r:id="rId29"/>
-    <hyperlink ref="H31" r:id="rId30"/>
-    <hyperlink ref="H32" r:id="rId31"/>
-    <hyperlink ref="H33" r:id="rId32"/>
-    <hyperlink ref="H34" r:id="rId33"/>
-    <hyperlink ref="H35" r:id="rId34"/>
-    <hyperlink ref="H36" r:id="rId35"/>
-    <hyperlink ref="H37" r:id="rId36"/>
-    <hyperlink ref="H38" r:id="rId37"/>
-    <hyperlink ref="H39" r:id="rId38"/>
-    <hyperlink ref="H40" r:id="rId39"/>
-    <hyperlink ref="H41" r:id="rId40"/>
-    <hyperlink ref="H42" r:id="rId41"/>
-    <hyperlink ref="H43" r:id="rId42"/>
-    <hyperlink ref="H44" r:id="rId43"/>
-    <hyperlink ref="H45" r:id="rId44"/>
-    <hyperlink ref="H46" r:id="rId45"/>
-    <hyperlink ref="H47" r:id="rId46"/>
-    <hyperlink ref="H48" r:id="rId47"/>
-    <hyperlink ref="H49" r:id="rId48"/>
-    <hyperlink ref="H50" r:id="rId49"/>
-    <hyperlink ref="H51" r:id="rId50"/>
-    <hyperlink ref="H52" r:id="rId51"/>
-    <hyperlink ref="H53" r:id="rId52"/>
-    <hyperlink ref="H54" r:id="rId53"/>
-    <hyperlink ref="H55" r:id="rId54"/>
-    <hyperlink ref="H56" r:id="rId55"/>
-    <hyperlink ref="H57" r:id="rId56"/>
-    <hyperlink ref="H58" r:id="rId57"/>
-    <hyperlink ref="H59" r:id="rId58"/>
-    <hyperlink ref="H60" r:id="rId59"/>
-    <hyperlink ref="H61" r:id="rId60"/>
-    <hyperlink ref="H62" r:id="rId61"/>
-    <hyperlink ref="H63" r:id="rId62"/>
-    <hyperlink ref="H64" r:id="rId63"/>
-    <hyperlink ref="H65" r:id="rId64"/>
-    <hyperlink ref="H66" r:id="rId65"/>
+    <hyperlink ref="H31" r:id="rId29"/>
+    <hyperlink ref="H32" r:id="rId30"/>
+    <hyperlink ref="H33" r:id="rId31"/>
+    <hyperlink ref="H34" r:id="rId32"/>
+    <hyperlink ref="H35" r:id="rId33"/>
+    <hyperlink ref="H36" r:id="rId34"/>
+    <hyperlink ref="H37" r:id="rId35"/>
+    <hyperlink ref="H38" r:id="rId36"/>
+    <hyperlink ref="H39" r:id="rId37"/>
+    <hyperlink ref="H40" r:id="rId38"/>
+    <hyperlink ref="H41" r:id="rId39"/>
+    <hyperlink ref="H42" r:id="rId40"/>
+    <hyperlink ref="H43" r:id="rId41"/>
+    <hyperlink ref="H44" r:id="rId42"/>
+    <hyperlink ref="H45" r:id="rId43"/>
+    <hyperlink ref="H46" r:id="rId44"/>
+    <hyperlink ref="H47" r:id="rId45"/>
+    <hyperlink ref="H48" r:id="rId46"/>
+    <hyperlink ref="H49" r:id="rId47"/>
+    <hyperlink ref="H50" r:id="rId48"/>
+    <hyperlink ref="H51" r:id="rId49"/>
+    <hyperlink ref="H52" r:id="rId50"/>
+    <hyperlink ref="H53" r:id="rId51"/>
+    <hyperlink ref="H54" r:id="rId52"/>
+    <hyperlink ref="H55" r:id="rId53"/>
+    <hyperlink ref="H56" r:id="rId54"/>
+    <hyperlink ref="H57" r:id="rId55"/>
+    <hyperlink ref="H58" r:id="rId56"/>
+    <hyperlink ref="H59" r:id="rId57"/>
+    <hyperlink ref="H60" r:id="rId58"/>
+    <hyperlink ref="H61" r:id="rId59"/>
+    <hyperlink ref="H62" r:id="rId60"/>
+    <hyperlink ref="H63" r:id="rId61"/>
+    <hyperlink ref="H64" r:id="rId62"/>
+    <hyperlink ref="H65" r:id="rId63"/>
+    <hyperlink ref="H66" r:id="rId64"/>
+    <hyperlink ref="H29" r:id="rId65"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>